<commit_message>
Assignp aram value even if prior is available
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF58C4A-AD69-064A-AD4C-1429434603E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00A4CE0-A402-C245-9FBC-8BF1B13B0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-600" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="-29400" yWindow="3240" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,6 +601,9 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
       <c r="C10" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Save UN population prospects data (population and deaths)
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DACF2DE-7F6B-384B-80E8-090F31FEAD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1EABAD-422A-F146-9C05-A0A78BBCF578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="20780" activeTab="1" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -739,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02B04A7-A509-3D48-B387-03DC52E1D6FB}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Forgot to push new infectiousness param
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594F2106-0EA0-8747-A9B6-CD50CB524AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C52E541-A6C9-4E44-921B-C7A47629ADC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29400" yWindow="3240" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>parameter</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>test_param</t>
+  </si>
+  <si>
+    <t>rel_infectiousness_subclin</t>
   </si>
 </sst>
 </file>
@@ -512,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,6 +749,14 @@
       </c>
       <c r="G22" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restore full analysis runner
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C52E541-A6C9-4E44-921B-C7A47629ADC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BAF8DE-39B8-9046-9DE1-DB984C453E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29400" yWindow="3240" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
+    <sheetView zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02B04A7-A509-3D48-B387-03DC52E1D6FB}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Detection adjusted by clinical status
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B64383-C926-7344-A7EF-93BA15C5D4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B8A1C9-24A6-CC47-BA9B-8E11BE6C9BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="1860" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>parameter</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>mixing_factor_ca</t>
+  </si>
+  <si>
+    <t>rel_detection_clinical</t>
   </si>
 </sst>
 </file>
@@ -524,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -790,6 +793,23 @@
       </c>
       <c r="B26">
         <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Target for prev infectious TB
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E49C273-657B-3D4C-92DB-FAB71541E0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C115204C-65A3-9049-9BBF-477F0405D99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>parameter</t>
   </si>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,7 +579,7 @@
         <v>0.5</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -605,6 +605,15 @@
       <c r="B5">
         <v>1</v>
       </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -750,6 +759,15 @@
       </c>
       <c r="B21">
         <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Full scale massive run
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C115204C-65A3-9049-9BBF-477F0405D99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF65F5B-F625-4340-A8A5-4C0005779934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="225" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,7 +579,7 @@
         <v>0.5</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -693,7 +693,7 @@
         <v>0.1</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -723,7 +723,7 @@
         <v>25</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>50</v>
@@ -767,7 +767,7 @@
         <v>0.5</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Major refactor of treatment outcomes
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC3B9B9-8261-3A43-9B2C-5B4130AFFA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FB793A-3591-FF40-8EA1-842785077D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>parameter</t>
   </si>
@@ -60,9 +60,6 @@
     <t>clinical_progression_rate</t>
   </si>
   <si>
-    <t>tx_death_rate</t>
-  </si>
-  <si>
     <t>tb_mortality_rate_inf</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>rel_sus_recovered</t>
   </si>
   <si>
-    <t>tx_recovery_rate</t>
-  </si>
-  <si>
     <t>clearance_rate</t>
   </si>
   <si>
@@ -105,9 +99,6 @@
     <t>clinical_regression_rate</t>
   </si>
   <si>
-    <t>tx_relapse_rate</t>
-  </si>
-  <si>
     <t>infectiousness_gain_rate</t>
   </si>
   <si>
@@ -117,9 +108,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>test_param</t>
-  </si>
-  <si>
     <t>rel_infectiousness_subclin</t>
   </si>
   <si>
@@ -205,6 +193,30 @@
   </si>
   <si>
     <t>\psi_{loss}</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>pct_neg_tx_death</t>
+  </si>
+  <si>
+    <t>tx_success_pct</t>
+  </si>
+  <si>
+    <t>tx_duration</t>
+  </si>
+  <si>
+    <t>\tau</t>
+  </si>
+  <si>
+    <t>average TB treatment duration</t>
+  </si>
+  <si>
+    <t>death fraction among negative treatment outcomes</t>
+  </si>
+  <si>
+    <t>annual TB detection rate in 2020</t>
   </si>
 </sst>
 </file>
@@ -283,13 +295,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -634,63 +644,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.83203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.83203125" style="5"/>
+    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>34</v>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -699,176 +708,176 @@
         <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="6">
+    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5">
         <v>0.1</v>
       </c>
-      <c r="E5" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="E10" s="5">
+        <v>3</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="I10" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="5">
+        <v>5</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="E7" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="B13" s="5">
         <v>0.1</v>
       </c>
-      <c r="E10" s="7">
-        <v>3</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="7">
-        <v>5</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="H12" s="7" t="s">
+      <c r="H13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>35</v>
+      <c r="I13" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -879,7 +888,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D14" s="3">
         <v>0.5</v>
@@ -888,35 +897,35 @@
         <v>10</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D16" s="3">
         <v>0.5</v>
@@ -925,153 +934,154 @@
         <v>10</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
       </c>
       <c r="H17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="7">
+        <v>10</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="8">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="E18" s="8">
+      <c r="B22" s="7">
         <v>0.5</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="8">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="E19" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="9">
-        <v>1</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="9">
+      <c r="G22" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="7">
+        <v>10</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47">
+        <v>0.5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47">
         <v>0.1</v>
       </c>
-      <c r="E21" s="9">
-        <v>10</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="9">
-        <v>2</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B48" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="E48" s="5">
+      <c r="E47">
         <v>1</v>
       </c>
     </row>
@@ -1086,28 +1096,29 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1900</v>
+        <v>1945</v>
       </c>
       <c r="B2">
-        <v>100000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1115,7 +1126,7 @@
         <v>1950</v>
       </c>
       <c r="B3">
-        <v>120000</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1123,7 +1134,7 @@
         <v>2000</v>
       </c>
       <c r="B4">
-        <v>189000</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1131,7 +1142,7 @@
         <v>2025</v>
       </c>
       <c r="B5">
-        <v>200000</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement raw version of ACF and TPT
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FB793A-3591-FF40-8EA1-842785077D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FCC4AC-7A74-9B4A-8B39-3004B3B0C58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -647,7 +647,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1096,7 +1096,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Compute prevalence using sensitivities
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FCC4AC-7A74-9B4A-8B39-3004B3B0C58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED04873-AA38-B44F-9577-D33ECBA7FE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>parameter</t>
   </si>
@@ -217,6 +217,30 @@
   </si>
   <si>
     <t>annual TB detection rate in 2020</t>
+  </si>
+  <si>
+    <t>comp-specific sensitivity during prevalence survey</t>
+  </si>
+  <si>
+    <t>prev_se_incipient</t>
+  </si>
+  <si>
+    <t>prev_se_contained</t>
+  </si>
+  <si>
+    <t>prev_se_cleared</t>
+  </si>
+  <si>
+    <t>prev_se_subclin_noninf</t>
+  </si>
+  <si>
+    <t>prev_se_clin_noninf</t>
+  </si>
+  <si>
+    <t>prev_se_subclin_inf</t>
+  </si>
+  <si>
+    <t>prev_se_clin_inf</t>
   </si>
 </sst>
 </file>
@@ -295,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -304,6 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1067,6 +1092,107 @@
       <c r="I23" s="7" t="s">
         <v>52</v>
       </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="8">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="8">
+        <v>1</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="8">
+        <v>1</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="8">
+        <v>1</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="8">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">

</xml_diff>

<commit_message>
Use sensible se parameters
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED04873-AA38-B44F-9577-D33ECBA7FE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AAC266-F6DC-174F-A965-F493C5D2D0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="40400" yWindow="1860" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
   <si>
     <t>parameter</t>
   </si>
@@ -231,16 +231,31 @@
     <t>prev_se_cleared</t>
   </si>
   <si>
-    <t>prev_se_subclin_noninf</t>
-  </si>
-  <si>
-    <t>prev_se_clin_noninf</t>
-  </si>
-  <si>
-    <t>prev_se_subclin_inf</t>
-  </si>
-  <si>
-    <t>prev_se_clin_inf</t>
+    <t>tpt_completion_perc</t>
+  </si>
+  <si>
+    <t>prev_se_subclin_noninf_pearl</t>
+  </si>
+  <si>
+    <t>prev_se_clin_noninf_pearl</t>
+  </si>
+  <si>
+    <t>prev_se_subclin_inf_pearl</t>
+  </si>
+  <si>
+    <t>prev_se_clin_inf_pearl</t>
+  </si>
+  <si>
+    <t>prev_se_clin_noninf_cxr</t>
+  </si>
+  <si>
+    <t>prev_se_subclin_inf_cxr</t>
+  </si>
+  <si>
+    <t>prev_se_clin_inf_cxr</t>
+  </si>
+  <si>
+    <t>prev_se_subclin_noninf_cxr</t>
   </si>
 </sst>
 </file>
@@ -319,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -328,7 +343,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,13 +685,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -1097,14 +1111,10 @@
       <c r="A24" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="8">
-        <v>1</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8" t="s">
+      <c r="B24">
+        <v>0.75</v>
+      </c>
+      <c r="G24" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1112,87 +1122,98 @@
       <c r="A25" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="8">
-        <v>1</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="B25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="8">
-        <v>1</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
+      <c r="B26">
+        <v>0.35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26">
+        <v>0.2</v>
+      </c>
+      <c r="E26">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="8">
-        <v>1</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
+        <v>65</v>
+      </c>
+      <c r="B27">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="8">
-        <v>1</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
+        <v>66</v>
+      </c>
+      <c r="B28">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="8">
-        <v>1</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
+        <v>67</v>
+      </c>
+      <c r="B29">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="8">
-        <v>1</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
+        <v>68</v>
+      </c>
+      <c r="B30">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">

</xml_diff>

<commit_message>
Refine params and calibration
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AAC266-F6DC-174F-A965-F493C5D2D0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8183F7B7-C6D1-F94B-B65F-9A6810B484BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40400" yWindow="1860" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="38400" yWindow="1860" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
     <sheet name="time_variant" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
   <si>
     <t>parameter</t>
   </si>
@@ -683,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -783,10 +783,10 @@
         <v>21</v>
       </c>
       <c r="D5" s="4">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="4">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>36</v>
@@ -806,7 +806,7 @@
         <v>0.5</v>
       </c>
       <c r="E6" s="4">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>37</v>
@@ -826,7 +826,7 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="4">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>38</v>
@@ -865,10 +865,10 @@
         <v>21</v>
       </c>
       <c r="D10" s="5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="E10" s="5">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>41</v>
@@ -884,6 +884,15 @@
       <c r="B11" s="5">
         <v>5</v>
       </c>
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>10</v>
+      </c>
       <c r="H11" s="5" t="s">
         <v>42</v>
       </c>
@@ -898,6 +907,15 @@
       <c r="B12" s="5">
         <v>0.1</v>
       </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
       <c r="H12" s="5" t="s">
         <v>43</v>
       </c>
@@ -910,7 +928,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>47</v>
@@ -1000,15 +1018,6 @@
       <c r="B18" s="6">
         <v>0.38900000000000001</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0.5</v>
-      </c>
       <c r="H18" s="6" t="s">
         <v>45</v>
       </c>
@@ -1023,15 +1032,6 @@
       <c r="B19" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="E19" s="6">
-        <v>0.04</v>
-      </c>
       <c r="H19" s="6" t="s">
         <v>46</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -1215,21 +1215,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>26</v>
       </c>
-      <c r="B47">
-        <v>0.5</v>
-      </c>
-      <c r="C47" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47">
-        <v>0.1</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
+      <c r="B36">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1243,7 +1234,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update Tx detah outcome using WHO data
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FAA4EB-6417-8640-9C1E-77DE6EEB4D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925D41FB-80E6-4B4B-A2D0-46EFABF62745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="1860" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1098,7 +1098,7 @@
         <v>53</v>
       </c>
       <c r="B23" s="7">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Refactor infectiousness dimension, noninf become lowinf
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925D41FB-80E6-4B4B-A2D0-46EFABF62745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2D70CA-7527-C04C-8BE7-209EC34716E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="1860" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
   <si>
     <t>parameter</t>
   </si>
@@ -69,9 +69,6 @@
     <t>rel_sus_cleared</t>
   </si>
   <si>
-    <t>tb_mortality_rate_noninf</t>
-  </si>
-  <si>
     <t>rel_sus_recovered</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>\mu_{TBinf}</t>
   </si>
   <si>
-    <t>\mu_{TBnoninf}</t>
-  </si>
-  <si>
     <t>\phi</t>
   </si>
   <si>
@@ -234,28 +228,37 @@
     <t>tpt_completion_perc</t>
   </si>
   <si>
-    <t>prev_se_subclin_noninf_pearl</t>
-  </si>
-  <si>
-    <t>prev_se_clin_noninf_pearl</t>
-  </si>
-  <si>
     <t>prev_se_subclin_inf_pearl</t>
   </si>
   <si>
     <t>prev_se_clin_inf_pearl</t>
   </si>
   <si>
-    <t>prev_se_clin_noninf_cxr</t>
-  </si>
-  <si>
     <t>prev_se_subclin_inf_cxr</t>
   </si>
   <si>
     <t>prev_se_clin_inf_cxr</t>
   </si>
   <si>
-    <t>prev_se_subclin_noninf_cxr</t>
+    <t>rel_infectiousness_lowinf</t>
+  </si>
+  <si>
+    <t>tb_mortality_rate_lowinf</t>
+  </si>
+  <si>
+    <t>\mu_{TBlowinf}</t>
+  </si>
+  <si>
+    <t>prev_se_subclin_lowinf_pearl</t>
+  </si>
+  <si>
+    <t>prev_se_clin_lowinf_pearl</t>
+  </si>
+  <si>
+    <t>prev_se_subclin_lowinf_cxr</t>
+  </si>
+  <si>
+    <t>prev_se_clin_lowinf_cxr</t>
   </si>
 </sst>
 </file>
@@ -683,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,24 +724,24 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -747,29 +750,29 @@
         <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -780,7 +783,7 @@
         <v>0.2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4">
         <v>0.2</v>
@@ -789,7 +792,7 @@
         <v>0.5</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -800,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4">
         <v>0.5</v>
@@ -809,18 +812,18 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4">
         <v>0.5</v>
@@ -829,268 +832,259 @@
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4">
         <v>0.5</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4">
         <v>0.5</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>31</v>
+    </row>
+    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B11" s="5">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="5">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="E11" s="5">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B12" s="5">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="5">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="E12" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5">
         <v>0.02</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E14" s="3">
-        <v>10</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>31</v>
+      <c r="H14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
       </c>
+      <c r="C15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="3">
+        <v>10</v>
+      </c>
       <c r="H15" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E16" s="3">
-        <v>10</v>
-      </c>
       <c r="H16" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
       </c>
+      <c r="C17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="3">
+        <v>10</v>
+      </c>
       <c r="H17" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="6">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B19" s="6">
-        <v>2.5000000000000001E-2</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="B20" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="6">
         <v>0.4</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="7">
-        <v>1</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E21" s="7">
-        <v>10</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>31</v>
+      <c r="H21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B22" s="7">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E22" s="7">
+        <v>10</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="I22" s="7" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1098,62 +1092,71 @@
         <v>53</v>
       </c>
       <c r="B23" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="7">
         <v>50</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24">
-        <v>0.75</v>
-      </c>
-      <c r="G24" t="s">
-        <v>60</v>
+      <c r="G24" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>0.75</v>
       </c>
+      <c r="G25" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B26">
-        <v>0.35</v>
-      </c>
-      <c r="C26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26">
-        <v>0.2</v>
-      </c>
-      <c r="E26">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B27">
-        <v>0.95</v>
+        <v>0.35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27">
+        <v>0.2</v>
+      </c>
+      <c r="E27">
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B28">
         <v>0.95</v>
@@ -1161,7 +1164,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B29">
         <v>0.95</v>
@@ -1169,7 +1172,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B30">
         <v>0.95</v>
@@ -1180,46 +1183,54 @@
         <v>64</v>
       </c>
       <c r="B31">
-        <v>70</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B32">
-        <v>0.5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B33">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B34">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B35">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="B36">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37">
         <v>0</v>
       </c>
     </row>
@@ -1245,10 +1256,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Refactor TB infection dynamics
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2D70CA-7527-C04C-8BE7-209EC34716E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D032C3CE-6105-3040-81D1-E1FE281D7DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="1860" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>parameter</t>
   </si>
@@ -78,9 +78,6 @@
     <t>infectiousness_loss_rate</t>
   </si>
   <si>
-    <t>progression_rate</t>
-  </si>
-  <si>
     <t>breakdown_rate</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>raw_transmission_rate</t>
   </si>
   <si>
-    <t>containment_rate</t>
-  </si>
-  <si>
     <t>clinical_regression_rate</t>
   </si>
   <si>
@@ -259,6 +253,24 @@
   </si>
   <si>
     <t>prev_se_clin_lowinf_cxr</t>
+  </si>
+  <si>
+    <t>progression_rate_age0</t>
+  </si>
+  <si>
+    <t>progression_rate_age5</t>
+  </si>
+  <si>
+    <t>progression_rate_age15</t>
+  </si>
+  <si>
+    <t>containment_rate_age0</t>
+  </si>
+  <si>
+    <t>containment_rate_age5</t>
+  </si>
+  <si>
+    <t>containment_rate_age15</t>
   </si>
 </sst>
 </file>
@@ -686,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -724,24 +736,24 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -750,29 +762,29 @@
         <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -783,7 +795,7 @@
         <v>0.2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4">
         <v>0.2</v>
@@ -792,7 +804,7 @@
         <v>0.5</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -803,7 +815,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4">
         <v>0.5</v>
@@ -812,7 +824,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -823,7 +835,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" s="4">
         <v>0.5</v>
@@ -832,23 +844,23 @@
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" s="4">
         <v>0.5</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4">
         <v>0.5</v>
@@ -856,381 +868,404 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B10" s="4">
         <v>0.4</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="B11" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0.5</v>
+        <v>2.4</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="B12" s="5">
-        <v>5</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5">
-        <v>10</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="B13" s="5">
         <v>0.1</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="E13" s="5">
-        <v>1</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="5">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B18" s="5">
         <v>0.02</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="C18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="3">
+        <v>10</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3">
+      <c r="I20" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3">
         <v>1</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="3">
+      <c r="C21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="3">
         <v>0.5</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E21" s="3">
         <v>10</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="I21" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="D26" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="7">
+        <v>10</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I27" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="3">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E17" s="3">
-        <v>10</v>
-      </c>
-      <c r="H17" s="3" t="s">
+    </row>
+    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="7">
+        <v>40</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="6">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="6">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="7">
-        <v>1</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E22" s="7">
-        <v>10</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="7">
-        <v>50</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25">
-        <v>0.75</v>
-      </c>
-      <c r="G25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27">
-        <v>0.35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27">
-        <v>0.2</v>
-      </c>
-      <c r="E27">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28">
-        <v>0.95</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B29">
-        <v>0.95</v>
+        <v>0.75</v>
+      </c>
+      <c r="G29" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B30">
-        <v>0.95</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B31">
-        <v>0.95</v>
+        <v>0.35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <v>0.2</v>
+      </c>
+      <c r="E31">
+        <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B32">
-        <v>70</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B33">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B34">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B35">
-        <v>0.6</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B36">
-        <v>0.9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="B37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41">
         <v>0</v>
       </c>
     </row>
@@ -1256,10 +1291,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Split progression between inf and lowinf
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D032C3CE-6105-3040-81D1-E1FE281D7DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3313D19A-7668-284E-8573-07B0A1BF94E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="1860" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="3480" yWindow="600" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
   <si>
     <t>parameter</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>containment_rate_age15</t>
+  </si>
+  <si>
+    <t>progression_prop_infectious</t>
   </si>
 </sst>
 </file>
@@ -698,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,10 +759,10 @@
         <v>18</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E2" s="2">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>30</v>
@@ -909,63 +912,48 @@
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B14" s="5">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>28</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="5">
         <v>4.4000000000000004</v>
       </c>
+      <c r="H15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="5">
-        <v>2</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B17" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="E17" s="5">
-        <v>1</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B18" s="5">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>18</v>
@@ -974,47 +962,56 @@
         <v>0.01</v>
       </c>
       <c r="E18" s="5">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
+    <row r="19" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E19" s="3">
-        <v>10</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="3" t="s">
+      <c r="D19" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
       </c>
+      <c r="C20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="3">
+        <v>5</v>
+      </c>
       <c r="H20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>28</v>
@@ -1022,22 +1019,13 @@
     </row>
     <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="3">
         <v>1</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E21" s="3">
-        <v>10</v>
-      </c>
       <c r="H21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>28</v>
@@ -1045,41 +1033,50 @@
     </row>
     <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
       </c>
+      <c r="C22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="3">
+        <v>5</v>
+      </c>
       <c r="H22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="6">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" s="6" t="s">
+    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="B24" s="6">
-        <v>2.5000000000000001E-2</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>28</v>
@@ -1087,119 +1084,125 @@
     </row>
     <row r="25" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="B25" s="6">
-        <v>0.4</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="7">
-        <v>1</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E26" s="7">
-        <v>10</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I26" s="7" t="s">
+    <row r="26" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B27" s="7">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E27" s="7">
+        <v>5</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B29" s="7">
         <v>40</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I29" s="7" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29">
-        <v>0.75</v>
-      </c>
-      <c r="G29" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30">
         <v>0.75</v>
       </c>
+      <c r="G30" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31">
-        <v>0.35</v>
-      </c>
-      <c r="C31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31">
-        <v>0.2</v>
-      </c>
-      <c r="E31">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B32">
-        <v>0.95</v>
+        <v>0.35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32">
+        <v>0.2</v>
+      </c>
+      <c r="E32">
+        <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33">
         <v>0.95</v>
@@ -1207,7 +1210,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B34">
         <v>0.95</v>
@@ -1215,7 +1218,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35">
         <v>0.95</v>
@@ -1223,49 +1226,57 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B36">
-        <v>70</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37">
         <v>70</v>
-      </c>
-      <c r="B37">
-        <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B38">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B39">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>23</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Use WHO tsr data
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3313D19A-7668-284E-8573-07B0A1BF94E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD918AB-E288-5B48-9D27-557BFBFE8F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="600" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="3480" yWindow="600" windowWidth="29400" windowHeight="18360" activeTab="1" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -703,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -1288,19 +1288,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02B04A7-A509-3D48-B387-03DC52E1D6FB}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1312,7 +1313,7 @@
       <c r="A2" s="1">
         <v>1945</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1320,27 +1321,222 @@
       <c r="A3" s="1">
         <v>1950</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>2000</v>
-      </c>
-      <c r="B4">
-        <v>75</v>
+        <v>1995</v>
+      </c>
+      <c r="B4" s="1">
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>2025</v>
-      </c>
-      <c r="B5">
+        <v>1998</v>
+      </c>
+      <c r="B5" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B6" s="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B8" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B9" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B10" s="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B11" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B12" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B13" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B14" s="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B15" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B16" s="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B17" s="1">
         <v>90</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B18" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B19" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B20" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B21" s="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B22" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B23" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B24" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B25" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B26" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B27" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B28" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B29" s="1">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B31">
+    <sortCondition ref="A2:A31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More progress on Quarto report
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89C10B3-D4B3-F44D-8B6D-90369675BE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AD6727-1270-9A4E-8339-503647E1A86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1060" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="104">
   <si>
     <t>parameter</t>
   </si>
@@ -198,15 +198,6 @@
     <t>\tau</t>
   </si>
   <si>
-    <t>average TB treatment duration</t>
-  </si>
-  <si>
-    <t>death fraction among negative treatment outcomes</t>
-  </si>
-  <si>
-    <t>annual TB detection rate in 2020</t>
-  </si>
-  <si>
     <t>comp-specific sensitivity during prevalence survey</t>
   </si>
   <si>
@@ -274,6 +265,90 @@
   </si>
   <si>
     <t>progression_prop_infectious</t>
+  </si>
+  <si>
+    <t>Effective rate of transmission (before adjusting for infectiousness)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Child-child mixing, relative to adult-adult mixing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Child-adult mixing, relative to adult-adult mixing</t>
+  </si>
+  <si>
+    <t>Rel. risk of reinfection from 'contained' compartment (ref. 'mtb-naïve')</t>
+  </si>
+  <si>
+    <t>Rel. susceptibility to infection for under 15 year-old individuals (ref. 15 and over)</t>
+  </si>
+  <si>
+    <t>Rel. risk of reinfection from 'cleared' compartment (ref. 'mtb-naïve')</t>
+  </si>
+  <si>
+    <t>Rel. risk of reinfection from 'recovered' compartment (ref. 'mtb-naïve')</t>
+  </si>
+  <si>
+    <t>Rel. infectiousness of subclinical TB (ref. clinical TB)</t>
+  </si>
+  <si>
+    <t>Rel. infectiousness of 'less infectious' TB (ref. 'more infectious' TB)</t>
+  </si>
+  <si>
+    <t>Rate of progression from 'incipient' to TB disease (age 0-4)</t>
+  </si>
+  <si>
+    <t>Rate of progression from 'incipient' to TB disease (age 5-14)</t>
+  </si>
+  <si>
+    <t>Rate of progression from 'incipient' to TB disease (age 15 and over)</t>
+  </si>
+  <si>
+    <t>Proportion of incident TB that is 'more infectious'</t>
+  </si>
+  <si>
+    <t>Rate of transition from 'incipient' to 'contained' (age 0-4)</t>
+  </si>
+  <si>
+    <t>Rate of transition from 'incipient' to 'contained' (age 5-14)</t>
+  </si>
+  <si>
+    <t>Rate of transition from 'incipient' to 'contained' (age 15 and over)</t>
+  </si>
+  <si>
+    <t>Rate of transition from 'contained' to 'incipient' (all ages)</t>
+  </si>
+  <si>
+    <t>Rate of transition from 'contained' to 'cleared' (all ages)</t>
+  </si>
+  <si>
+    <t>Rate of progression from subclinical to clinical TB</t>
+  </si>
+  <si>
+    <t>Rate of transition from clinical to subclinical TB</t>
+  </si>
+  <si>
+    <t>Rate of progression from 'less infectious' to 'more infectious' TB</t>
+  </si>
+  <si>
+    <t>Rate of transition from 'more infectious' to 'less infectious' TB</t>
+  </si>
+  <si>
+    <t>Rate of TB mortality for 'more infectious' clinical disease</t>
+  </si>
+  <si>
+    <t>Rate of TB mortality for 'less infectious' clinical disease</t>
+  </si>
+  <si>
+    <t>Rate of self-recovery for subclinical TB</t>
+  </si>
+  <si>
+    <t>Annual rate of TB detection in 2020</t>
+  </si>
+  <si>
+    <t>Average TB treatment duration</t>
+  </si>
+  <si>
+    <t>Percentage of deaths among negative TB treatment outcomes</t>
   </si>
 </sst>
 </file>
@@ -703,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,7 +789,7 @@
     <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="66.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -764,6 +839,9 @@
       <c r="E2" s="2">
         <v>10</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="H2" s="2" t="s">
         <v>30</v>
       </c>
@@ -775,6 +853,9 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="H3" s="2" t="s">
         <v>31</v>
       </c>
@@ -786,6 +867,9 @@
       <c r="B4" s="2">
         <v>1</v>
       </c>
+      <c r="G4" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="H4" s="2" t="s">
         <v>32</v>
       </c>
@@ -806,6 +890,9 @@
       <c r="E5" s="4">
         <v>0.5</v>
       </c>
+      <c r="G5" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="H5" s="4" t="s">
         <v>33</v>
       </c>
@@ -826,6 +913,9 @@
       <c r="E6" s="4">
         <v>1</v>
       </c>
+      <c r="G6" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="H6" s="4" t="s">
         <v>34</v>
       </c>
@@ -846,6 +936,9 @@
       <c r="E7" s="4">
         <v>1</v>
       </c>
+      <c r="G7" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="H7" s="4" t="s">
         <v>35</v>
       </c>
@@ -857,6 +950,9 @@
       <c r="B8" s="4">
         <v>0.5</v>
       </c>
+      <c r="G8" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="H8" s="4" t="s">
         <v>36</v>
       </c>
@@ -868,25 +964,34 @@
       <c r="B9" s="4">
         <v>0.5</v>
       </c>
+      <c r="G9" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B10" s="4">
         <v>0.4</v>
       </c>
+      <c r="G10" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="H10" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B11" s="5">
         <v>2.4</v>
       </c>
+      <c r="G11" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="H11" s="5" t="s">
         <v>38</v>
       </c>
@@ -896,35 +1001,47 @@
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B12" s="5">
         <v>2</v>
       </c>
+      <c r="G12" s="5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B13" s="5">
         <v>0.1</v>
       </c>
+      <c r="G13" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B14" s="5">
         <v>0.5</v>
       </c>
+      <c r="G14" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B15" s="5">
         <v>4.4000000000000004</v>
       </c>
+      <c r="G15" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="H15" s="5" t="s">
         <v>39</v>
       </c>
@@ -934,18 +1051,24 @@
     </row>
     <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B16" s="5">
         <v>4.4000000000000004</v>
       </c>
+      <c r="G16" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B17" s="5">
         <v>2</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -964,6 +1087,9 @@
       <c r="E18" s="5">
         <v>1</v>
       </c>
+      <c r="G18" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="H18" s="5" t="s">
         <v>40</v>
       </c>
@@ -987,6 +1113,9 @@
       <c r="E19" s="5">
         <v>0.03</v>
       </c>
+      <c r="G19" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="H19" s="5" t="s">
         <v>43</v>
       </c>
@@ -1010,6 +1139,9 @@
       <c r="E20" s="3">
         <v>5</v>
       </c>
+      <c r="G20" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="H20" s="3" t="s">
         <v>44</v>
       </c>
@@ -1024,6 +1156,9 @@
       <c r="B21" s="3">
         <v>1</v>
       </c>
+      <c r="G21" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="H21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1047,6 +1182,9 @@
       <c r="E22" s="3">
         <v>5</v>
       </c>
+      <c r="G22" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="H22" s="3" t="s">
         <v>46</v>
       </c>
@@ -1061,6 +1199,9 @@
       <c r="B23" s="3">
         <v>1</v>
       </c>
+      <c r="G23" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="H23" s="3" t="s">
         <v>47</v>
       </c>
@@ -1075,6 +1216,9 @@
       <c r="B24" s="6">
         <v>0.38900000000000001</v>
       </c>
+      <c r="G24" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="H24" s="6" t="s">
         <v>42</v>
       </c>
@@ -1084,13 +1228,16 @@
     </row>
     <row r="25" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B25" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
+      <c r="G25" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="H25" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>28</v>
@@ -1103,6 +1250,9 @@
       <c r="B26" s="6">
         <v>0.4</v>
       </c>
+      <c r="G26" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="H26" s="6" t="s">
         <v>41</v>
       </c>
@@ -1127,7 +1277,7 @@
         <v>5</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="I27" s="7" t="s">
         <v>28</v>
@@ -1141,7 +1291,7 @@
         <v>0.5</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>52</v>
@@ -1158,7 +1308,7 @@
         <v>40</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="I29" s="7" t="s">
         <v>48</v>
@@ -1166,18 +1316,18 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B30">
         <v>0.75</v>
       </c>
       <c r="G30" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B31">
         <v>0.75</v>
@@ -1185,7 +1335,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B32">
         <v>0.35</v>
@@ -1202,7 +1352,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B33">
         <v>0.95</v>
@@ -1210,7 +1360,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B34">
         <v>0.95</v>
@@ -1218,7 +1368,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B35">
         <v>0.95</v>
@@ -1226,7 +1376,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B36">
         <v>0.95</v>
@@ -1234,7 +1384,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B37">
         <v>70</v>
@@ -1242,7 +1392,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B38">
         <v>0.5</v>
@@ -1250,7 +1400,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B39">
         <v>0.9</v>
@@ -1258,7 +1408,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B40">
         <v>0.6</v>
@@ -1266,7 +1416,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B41">
         <v>0.9</v>

</xml_diff>

<commit_message>
Broader prior for clearance
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE33725-F523-6A44-9019-83FDB515D117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F4B513-D990-E847-BF4F-B23DFBD85D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -814,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1162,7 +1162,7 @@
         <v>0.01</v>
       </c>
       <c r="E19" s="5">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Use priors for CXR subclinical se parameters
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC193181-6381-A947-8B03-16F2A6FDE9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F887326-1FB2-7345-B2AA-68428AA3C711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="113">
   <si>
     <t>parameter</t>
   </si>
@@ -69,9 +69,6 @@
     <t>rel_sus_cleared</t>
   </si>
   <si>
-    <t>rel_sus_recovered</t>
-  </si>
-  <si>
     <t>clearance_rate</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>\sigma_{cleared}</t>
   </si>
   <si>
-    <t>\sigma_{recovered}</t>
-  </si>
-  <si>
     <t>\sigma_{child}</t>
   </si>
   <si>
@@ -280,9 +274,6 @@
   </si>
   <si>
     <t>Rel. risk of reinfection from 'cleared' compartment (ref. 'mtb-naïve')</t>
-  </si>
-  <si>
-    <t>Rel. risk of reinfection from 'recovered' compartment (ref. 'mtb-naïve')</t>
   </si>
   <si>
     <t>Rel. infectiousness of subclinical TB (ref. clinical TB)</t>
@@ -812,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView zoomScale="188" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -850,24 +841,24 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2">
         <v>0.1</v>
@@ -876,38 +867,38 @@
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -918,7 +909,7 @@
         <v>0.2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="4">
         <v>0.2</v>
@@ -927,10 +918,10 @@
         <v>0.5</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -941,7 +932,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4">
         <v>0.5</v>
@@ -950,38 +941,29 @@
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="4">
         <v>0.5</v>
       </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
       <c r="G7" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4">
         <v>0.5</v>
@@ -989,215 +971,218 @@
       <c r="G8" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B9" s="4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>37</v>
+        <v>80</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2.4</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="5">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="5">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B13" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B14" s="5">
-        <v>0.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="5">
-        <v>4.4000000000000004</v>
+        <v>2</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="B17" s="5">
-        <v>2</v>
+        <v>0.1</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B18" s="5">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="5">
         <v>0.01</v>
       </c>
       <c r="E18" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3">
         <v>1</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="E19" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>28</v>
+      <c r="C19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="3">
+        <v>5</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E20" s="3">
-        <v>5</v>
-      </c>
       <c r="G20" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1207,317 +1192,318 @@
       <c r="B21" s="3">
         <v>1</v>
       </c>
+      <c r="C21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="3">
+        <v>5</v>
+      </c>
       <c r="G21" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E22" s="3">
-        <v>5</v>
-      </c>
       <c r="G22" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="B24" s="6">
-        <v>0.38900000000000001</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="B25" s="6">
-        <v>2.5000000000000001E-2</v>
+        <v>0.4</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="7">
+        <v>5</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B27" s="7">
-        <v>1</v>
-      </c>
-      <c r="C27" s="7" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="D27" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E27" s="7">
-        <v>5</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="7">
+        <v>40</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="7">
-        <v>40</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>48</v>
+      <c r="B29">
+        <v>0.75</v>
+      </c>
+      <c r="G29" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30">
         <v>0.75</v>
       </c>
       <c r="G30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31">
-        <v>0.75</v>
+        <v>0.35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31">
+        <v>0.2</v>
+      </c>
+      <c r="E31">
+        <v>0.5</v>
       </c>
       <c r="G31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B32">
-        <v>0.35</v>
-      </c>
-      <c r="C32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32">
-        <v>0.2</v>
-      </c>
-      <c r="E32">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B33">
         <v>0.95</v>
       </c>
       <c r="G33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B34">
         <v>0.95</v>
       </c>
       <c r="G34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B35">
         <v>0.95</v>
       </c>
       <c r="G35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B36">
-        <v>0.95</v>
+        <v>70</v>
       </c>
       <c r="G36" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="I36" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B37">
-        <v>70</v>
+        <v>0.5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37">
+        <v>0.2</v>
+      </c>
+      <c r="E37">
+        <v>0.5</v>
       </c>
       <c r="G37" t="s">
-        <v>110</v>
-      </c>
-      <c r="I37" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B38">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G38" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B39">
-        <v>0.9</v>
+        <v>0.6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39">
+        <v>0.5</v>
+      </c>
+      <c r="E39">
+        <v>0.95</v>
       </c>
       <c r="G39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40">
-        <v>0.6</v>
+        <v>0.95</v>
       </c>
       <c r="G40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="B41">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="G42" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1530,7 +1516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02B04A7-A509-3D48-B387-03DC52E1D6FB}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -1543,10 +1529,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Major refactor of prevalence outputs for different tests
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F887326-1FB2-7345-B2AA-68428AA3C711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D252967-B03F-114D-812E-A311F717F8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -806,7 +806,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Include Tongue Swab, and Symptom Screening, now 25 scenarios
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D252967-B03F-114D-812E-A311F717F8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D190997-0757-B84E-86FB-09C7E5415971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="38400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="129">
   <si>
     <t>parameter</t>
   </si>
@@ -376,13 +376,61 @@
   </si>
   <si>
     <t>Relative detection rate of subclinical TB under passive case finding (ref. clinical TB)</t>
+  </si>
+  <si>
+    <t>prev_se_subclin_lowinf_plts</t>
+  </si>
+  <si>
+    <t>prev_se_clin_lowinf_plts</t>
+  </si>
+  <si>
+    <t>prev_se_subclin_inf_plts</t>
+  </si>
+  <si>
+    <t>prev_se_clin_inf_plts</t>
+  </si>
+  <si>
+    <t>Probability PLTS-positive for 'subclinical' and 'less infectious' category</t>
+  </si>
+  <si>
+    <t>Probability PLTS-positive for 'clinical' and 'less infectious' category</t>
+  </si>
+  <si>
+    <t>Probability PLTS-positive for 'subclinical' and 'more infectious' category</t>
+  </si>
+  <si>
+    <t>Probability PLTS-positive for 'clinical' and 'more infectious' category</t>
+  </si>
+  <si>
+    <t>prev_se_subclin_lowinf_ssx</t>
+  </si>
+  <si>
+    <t>prev_se_clin_lowinf_ssx</t>
+  </si>
+  <si>
+    <t>prev_se_subclin_inf_ssx</t>
+  </si>
+  <si>
+    <t>prev_se_clin_inf_ssx</t>
+  </si>
+  <si>
+    <t>Probability SSx-positive for 'subclinical' and 'less infectious' category</t>
+  </si>
+  <si>
+    <t>Probability SSx-positive for 'clinical' and 'less infectious' category</t>
+  </si>
+  <si>
+    <t>Probability SSx-positive for 'subclinical' and 'more infectious' category</t>
+  </si>
+  <si>
+    <t>Probability SSx-positive for 'clinical' and 'more infectious' category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,6 +443,41 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -454,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -463,6 +546,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1333,176 +1421,264 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="5">
         <v>0.75</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="5">
         <v>0.75</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="5">
         <v>0.35</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="5">
         <v>0.2</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="5">
         <v>0.5</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B32">
-        <v>0.95</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="B32" s="9">
+        <v>1</v>
+      </c>
+      <c r="G32" s="9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B33">
-        <v>0.95</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="B33" s="9">
+        <v>1</v>
+      </c>
+      <c r="G33" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B34">
-        <v>0.95</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="B34" s="9">
+        <v>1</v>
+      </c>
+      <c r="G34" s="9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B35">
-        <v>0.95</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="B35" s="9">
+        <v>1</v>
+      </c>
+      <c r="G35" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="10">
+        <v>1</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="10">
+        <v>1</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E40" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="11">
+        <v>1</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E42" s="11">
+        <v>1</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="11">
+        <v>1</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="12">
+        <v>0</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" s="12">
+        <v>1</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="12">
+        <v>0</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="12">
+        <v>1</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B36">
+      <c r="B48" s="8">
         <v>70</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G48" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I48" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37">
-        <v>0.5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37">
-        <v>0.2</v>
-      </c>
-      <c r="E37">
-        <v>0.5</v>
-      </c>
-      <c r="G37" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38">
-        <v>0.95</v>
-      </c>
-      <c r="G38" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39">
-        <v>0.6</v>
-      </c>
-      <c r="C39" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39">
-        <v>0.5</v>
-      </c>
-      <c r="E39">
-        <v>0.95</v>
-      </c>
-      <c r="G39" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40">
-        <v>0.95</v>
-      </c>
-      <c r="G40" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>22</v>
       </c>
-      <c r="B41">
+      <c r="B49">
         <v>0</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G49" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Use tanh to scale up detection
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D190997-0757-B84E-86FB-09C7E5415971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7157E381-F9C9-2346-83C6-71FB99CA94F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="38400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="133">
   <si>
     <t>parameter</t>
   </si>
@@ -424,6 +424,18 @@
   </si>
   <si>
     <t>Probability SSx-positive for 'clinical' and 'more infectious' category</t>
+  </si>
+  <si>
+    <t>Time when passive detection started to scale up</t>
+  </si>
+  <si>
+    <t>passive_detection_shape</t>
+  </si>
+  <si>
+    <t>Shape parameter of passive detection scale-up profile</t>
+  </si>
+  <si>
+    <t>passive_detection_inflection</t>
   </si>
 </sst>
 </file>
@@ -537,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -551,6 +563,8 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -891,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1680,6 +1694,48 @@
       </c>
       <c r="G49" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" s="13">
+        <v>2000</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="14">
+        <v>1990</v>
+      </c>
+      <c r="E50" s="14">
+        <v>2020</v>
+      </c>
+      <c r="F50" s="14"/>
+      <c r="G50" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>130</v>
+      </c>
+      <c r="B51" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="E51" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="F51" s="14"/>
+      <c r="G51" s="13" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revise pearl scenario definition
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7157E381-F9C9-2346-83C6-71FB99CA94F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331C0560-2D04-8748-B75A-26ACB49B952C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -549,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -563,8 +563,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1703,16 +1702,15 @@
       <c r="B50" s="13">
         <v>2000</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" t="s">
         <v>17</v>
       </c>
-      <c r="D50" s="14">
+      <c r="D50">
         <v>1990</v>
       </c>
-      <c r="E50" s="14">
+      <c r="E50">
         <v>2020</v>
       </c>
-      <c r="F50" s="14"/>
       <c r="G50" s="13" t="s">
         <v>129</v>
       </c>
@@ -1724,16 +1722,15 @@
       <c r="B51" s="13">
         <v>0.1</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="14">
+      <c r="D51">
         <v>0.05</v>
       </c>
-      <c r="E51" s="14">
+      <c r="E51">
         <v>0.2</v>
       </c>
-      <c r="F51" s="14"/>
       <c r="G51" s="13" t="s">
         <v>131</v>
       </c>

</xml_diff>

<commit_message>
Use density dependent transmission
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647B7EFD-B586-4746-8B1F-419190E43030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D030B85E-0727-694A-A6EC-BAC2841940F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -956,16 +956,16 @@
         <v>14</v>
       </c>
       <c r="B2" s="2">
-        <v>10</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="2">
-        <v>0.1</v>
+        <v>1E-4</v>
       </c>
       <c r="E2" s="2">
-        <v>10</v>
+        <v>1E-3</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
Switch back to frequency-dependent transmission for now
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D030B85E-0727-694A-A6EC-BAC2841940F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969C39E5-6FE8-3E44-AA0F-3DD4A78523C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -426,6 +426,9 @@
     <t>Probability SSx-positive for 'clinical' and 'more infectious' category</t>
   </si>
   <si>
+    <t>passive_detection_inflection</t>
+  </si>
+  <si>
     <t>Time when passive detection started to scale up</t>
   </si>
   <si>
@@ -433,9 +436,6 @@
   </si>
   <si>
     <t>Shape parameter of passive detection scale-up profile</t>
-  </si>
-  <si>
-    <t>passive_detection_inflection</t>
   </si>
 </sst>
 </file>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -956,16 +956,16 @@
         <v>14</v>
       </c>
       <c r="B2" s="2">
-        <v>2.0000000000000001E-4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="2">
-        <v>1E-4</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2">
-        <v>1E-3</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>73</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B50" s="13">
         <v>2000</v>
@@ -1712,12 +1712,12 @@
         <v>2020</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B51" s="13">
         <v>0.1</v>
@@ -1732,7 +1732,7 @@
         <v>0.2</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1746,7 +1746,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Calibrate passive detection trend
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969C39E5-6FE8-3E44-AA0F-3DD4A78523C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF98EE0C-A861-BF49-B6A5-88824AD8CA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="135">
   <si>
     <t>parameter</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t>Shape parameter of passive detection scale-up profile</t>
+  </si>
+  <si>
+    <t>passive_detection_past_frac</t>
+  </si>
+  <si>
+    <t>Past passive detection rate, as a fraction of the current one</t>
   </si>
 </sst>
 </file>
@@ -904,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD51"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1733,6 +1739,26 @@
       </c>
       <c r="G51" s="13" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B52">
+        <v>0.75</v>
+      </c>
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52">
+        <v>0.5</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="G52" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use generalised transmission mode in TB model
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF98EE0C-A861-BF49-B6A5-88824AD8CA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A3F9C5-080D-D44F-A2FD-C889B549D451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="136">
   <si>
     <t>parameter</t>
   </si>
@@ -442,6 +442,9 @@
   </si>
   <si>
     <t>Past passive detection rate, as a fraction of the current one</t>
+  </si>
+  <si>
+    <t>infection_pop_scale</t>
   </si>
 </sst>
 </file>
@@ -910,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -968,10 +971,10 @@
         <v>17</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="E2" s="2">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>73</v>
@@ -1759,6 +1762,14 @@
       </c>
       <c r="G52" t="s">
         <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Broaden priors for cxr se params
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F0E0C6-3058-B740-92F4-836FCF853AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C57B4F9-05EE-AC43-B56B-1A3A1A8FAE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="1920" yWindow="2160" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="137">
   <si>
     <t>parameter</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>infection_pop_scale</t>
+  </si>
+  <si>
+    <t>Exponent for population scaling in force of infection calculation</t>
   </si>
 </sst>
 </file>
@@ -915,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1587,7 +1590,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="11">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G40" s="11" t="s">
         <v>108</v>
@@ -1615,10 +1618,10 @@
         <v>17</v>
       </c>
       <c r="D42" s="11">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E42" s="11">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G42" s="11" t="s">
         <v>110</v>
@@ -1779,6 +1782,9 @@
       </c>
       <c r="E53">
         <v>1</v>
+      </c>
+      <c r="G53" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement heterogenous mixing using socialising params
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C57B4F9-05EE-AC43-B56B-1A3A1A8FAE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417976F7-1CD4-0E46-A6E5-3BD8CB2CF318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="2160" windowWidth="29400" windowHeight="18360" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="137">
   <si>
     <t>parameter</t>
   </si>
@@ -99,12 +99,6 @@
     <t>rel_infectiousness_subclin</t>
   </si>
   <si>
-    <t>mixing_factor_cc</t>
-  </si>
-  <si>
-    <t>mixing_factor_ca</t>
-  </si>
-  <si>
     <t>rel_detection_subclin</t>
   </si>
   <si>
@@ -261,12 +255,6 @@
     <t>Effective rate of transmission (before adjusting for infectiousness)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Child-child mixing, relative to adult-adult mixing</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Child-adult mixing, relative to adult-adult mixing</t>
-  </si>
-  <si>
     <t>Rel. risk of reinfection from 'contained' compartment (ref. 'mtb-naïve')</t>
   </si>
   <si>
@@ -448,6 +436,18 @@
   </si>
   <si>
     <t>Exponent for population scaling in force of infection calculation</t>
+  </si>
+  <si>
+    <t>child_socialising</t>
+  </si>
+  <si>
+    <t>elderly_socialising</t>
+  </si>
+  <si>
+    <t>Social activity level for 65+ years old (relative to 15-64 years-old)</t>
+  </si>
+  <si>
+    <t>Social activity level for 0-14 years old (relative to 15-64 years-old)</t>
   </si>
 </sst>
 </file>
@@ -918,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -954,13 +954,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -974,44 +974,62 @@
         <v>17</v>
       </c>
       <c r="D2" s="2">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-3</v>
       </c>
       <c r="E2" s="2">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>133</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
       <c r="G3" s="2" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
       <c r="G4" s="2" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1031,10 +1049,10 @@
         <v>0.5</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1054,24 +1072,24 @@
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4">
         <v>0.5</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1082,125 +1100,125 @@
         <v>0.5</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9" s="4">
         <v>0.4</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B10" s="5">
         <v>2.4</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" s="5">
         <v>2</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B12" s="5">
         <v>0.1</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B13" s="5">
         <v>0.5</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B15" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B16" s="5">
         <v>2</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1220,13 +1238,13 @@
         <v>1</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1246,13 +1264,13 @@
         <v>0.1</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1272,13 +1290,13 @@
         <v>5</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1289,13 +1307,13 @@
         <v>1</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1315,13 +1333,13 @@
         <v>5</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1332,13 +1350,13 @@
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1349,30 +1367,30 @@
         <v>0.38900000000000001</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B24" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1383,18 +1401,18 @@
         <v>0.4</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" s="7">
         <v>1</v>
@@ -1409,24 +1427,24 @@
         <v>5</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B27" s="7">
         <v>0.5</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I27" s="7" t="s">
         <v>18</v>
@@ -1434,43 +1452,43 @@
     </row>
     <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B28" s="7">
         <v>40</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B29" s="5">
         <v>0.75</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" s="5">
         <v>0.75</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B31" s="5">
         <v>0.35</v>
@@ -1485,100 +1503,100 @@
         <v>0.5</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B32" s="9">
         <v>1</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B34" s="9">
         <v>1</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B35" s="9">
         <v>1</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B36" s="10">
         <v>0.3</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="10">
+        <v>1</v>
+      </c>
+      <c r="G37" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="B37" s="10">
-        <v>1</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B38" s="10">
         <v>0.5</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="10">
+        <v>1</v>
+      </c>
+      <c r="G39" s="10" t="s">
         <v>116</v>
-      </c>
-      <c r="B39" s="10">
-        <v>1</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B40" s="11">
         <v>0.1</v>
@@ -1593,23 +1611,23 @@
         <v>0.5</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B41" s="11">
         <v>1</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B42" s="11">
         <v>0.4</v>
@@ -1624,92 +1642,92 @@
         <v>1</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B43" s="11">
         <v>1</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B44" s="12">
         <v>0</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="12">
+        <v>1</v>
+      </c>
+      <c r="G45" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="B45" s="12">
-        <v>1</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B46" s="12">
         <v>0</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" s="12">
+        <v>1</v>
+      </c>
+      <c r="G47" s="12" t="s">
         <v>124</v>
-      </c>
-      <c r="B47" s="12">
-        <v>1</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B48" s="8">
         <v>70</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B50" s="13">
         <v>2000</v>
@@ -1724,12 +1742,12 @@
         <v>2020</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B51" s="13">
         <v>0.1</v>
@@ -1744,12 +1762,12 @@
         <v>0.2</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B52">
         <v>0.75</v>
@@ -1764,12 +1782,12 @@
         <v>1</v>
       </c>
       <c r="G52" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B53">
         <v>0.5</v>
@@ -1784,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1813,7 +1831,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update prior for raw transmission rate
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417976F7-1CD4-0E46-A6E5-3BD8CB2CF318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E91DB9-7060-0D4C-A2A7-112CB318A77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -444,10 +444,10 @@
     <t>elderly_socialising</t>
   </si>
   <si>
-    <t>Social activity level for 65+ years old (relative to 15-64 years-old)</t>
-  </si>
-  <si>
-    <t>Social activity level for 0-14 years old (relative to 15-64 years-old)</t>
+    <t>Social activity level of 0-14 years old (relative to 15-64 years-old)</t>
+  </si>
+  <si>
+    <t>Social activity level of 65+ years old (relative to 15-64 years-old)</t>
   </si>
 </sst>
 </file>
@@ -919,7 +919,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -968,7 +968,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="2">
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>17</v>
@@ -977,7 +977,7 @@
         <v>1E-3</v>
       </c>
       <c r="E2" s="2">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>71</v>
@@ -1003,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>28</v>
@@ -1026,7 +1026,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Failing attempt to integrate new mixing into model
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E91DB9-7060-0D4C-A2A7-112CB318A77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5452F8-BBB8-0D49-84EE-4E1390FB52B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="135">
   <si>
     <t>parameter</t>
   </si>
@@ -438,16 +438,10 @@
     <t>Exponent for population scaling in force of infection calculation</t>
   </si>
   <si>
-    <t>child_socialising</t>
-  </si>
-  <si>
-    <t>elderly_socialising</t>
-  </si>
-  <si>
-    <t>Social activity level of 0-14 years old (relative to 15-64 years-old)</t>
-  </si>
-  <si>
-    <t>Social activity level of 65+ years old (relative to 15-64 years-old)</t>
+    <t>mixing_a_spread</t>
+  </si>
+  <si>
+    <t>mixing_pc_strength</t>
   </si>
 </sst>
 </file>
@@ -919,7 +913,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -991,19 +985,16 @@
         <v>133</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="2">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>28</v>
@@ -1020,13 +1011,10 @@
         <v>17</v>
       </c>
       <c r="D4" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>136</v>
+        <v>5</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Model now using new mixing model
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E91DB9-7060-0D4C-A2A7-112CB318A77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C96B78B-F169-3B4A-B96D-4FA29EB1493F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="1540" yWindow="2220" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="139">
   <si>
     <t>parameter</t>
   </si>
@@ -438,16 +438,22 @@
     <t>Exponent for population scaling in force of infection calculation</t>
   </si>
   <si>
-    <t>child_socialising</t>
-  </si>
-  <si>
-    <t>elderly_socialising</t>
-  </si>
-  <si>
-    <t>Social activity level of 0-14 years old (relative to 15-64 years-old)</t>
-  </si>
-  <si>
-    <t>Social activity level of 65+ years old (relative to 15-64 years-old)</t>
+    <t>a_spread</t>
+  </si>
+  <si>
+    <t>pc_strength</t>
+  </si>
+  <si>
+    <t>bg_mixing</t>
+  </si>
+  <si>
+    <t>Background age-agnostic mixing level</t>
+  </si>
+  <si>
+    <t>Spread of assortative mixing pattern (smaller value means more assortativity)</t>
+  </si>
+  <si>
+    <t>Strength of parent-children mixing pattern</t>
   </si>
 </sst>
 </file>
@@ -916,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,161 +994,167 @@
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="2">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="4">
         <v>0.5</v>
       </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4">
         <v>0.5</v>
       </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
       <c r="G7" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B8" s="4">
         <v>0.5</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="4">
         <v>0.4</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="5">
-        <v>2.4</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="5">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>25</v>
@@ -1150,13 +1162,13 @@
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="5">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>25</v>
@@ -1164,13 +1176,13 @@
     </row>
     <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B13" s="5">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>25</v>
@@ -1178,16 +1190,13 @@
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B14" s="5">
-        <v>4.4000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>25</v>
@@ -1195,13 +1204,16 @@
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>25</v>
@@ -1209,13 +1221,13 @@
     </row>
     <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16" s="5">
-        <v>2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>25</v>
@@ -1223,25 +1235,13 @@
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B17" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="E17" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>25</v>
@@ -1249,10 +1249,10 @@
     </row>
     <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B18" s="5">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>17</v>
@@ -1261,56 +1261,65 @@
         <v>0.01</v>
       </c>
       <c r="E18" s="5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
+    <row r="19" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E19" s="3">
-        <v>5</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="3" t="s">
+      <c r="D19" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
       </c>
+      <c r="C20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="3">
+        <v>5</v>
+      </c>
       <c r="G20" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>25</v>
@@ -1318,25 +1327,16 @@
     </row>
     <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="3">
         <v>1</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E21" s="3">
-        <v>5</v>
-      </c>
       <c r="G21" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>25</v>
@@ -1344,50 +1344,59 @@
     </row>
     <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
       </c>
+      <c r="C22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="3">
+        <v>5</v>
+      </c>
       <c r="G22" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="6">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="6" t="s">
+    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="B24" s="6">
-        <v>2.5000000000000001E-2</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>25</v>
@@ -1395,413 +1404,430 @@
     </row>
     <row r="25" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="B25" s="6">
-        <v>0.4</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="7">
-        <v>1</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E26" s="7">
-        <v>5</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I26" s="7" t="s">
+    <row r="26" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B27" s="7">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E27" s="7">
+        <v>5</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B29" s="7">
         <v>40</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I29" s="7" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" s="5">
         <v>0.75</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B32" s="5">
         <v>0.35</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D32" s="5">
         <v>0.2</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E32" s="5">
         <v>0.5</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
+    <row r="33" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="B32" s="9">
-        <v>1</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B34" s="9">
         <v>1</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" s="9">
         <v>1</v>
       </c>
       <c r="G35" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="9">
+        <v>1</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
+    <row r="37" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B37" s="10">
         <v>0.3</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G37" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+    <row r="38" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B38" s="10">
         <v>1</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G38" s="10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
+    <row r="39" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B39" s="10">
         <v>0.5</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="G39" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
+    <row r="40" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B40" s="10">
         <v>1</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="G40" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
+    <row r="41" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B41" s="11">
         <v>0.1</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C41" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D41" s="11">
         <v>0</v>
       </c>
-      <c r="E40" s="11">
+      <c r="E41" s="11">
         <v>0.5</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="G41" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
+    <row r="42" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B42" s="11">
         <v>1</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="G42" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
+    <row r="43" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="11">
+      <c r="B43" s="11">
         <v>0.4</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C43" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D43" s="11">
         <v>0.5</v>
       </c>
-      <c r="E42" s="11">
+      <c r="E43" s="11">
         <v>1</v>
       </c>
-      <c r="G42" s="11" t="s">
+      <c r="G43" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
+    <row r="44" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="11">
+      <c r="B44" s="11">
         <v>1</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="G44" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="12" t="s">
+    <row r="45" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B45" s="12">
         <v>0</v>
       </c>
-      <c r="G44" s="12" t="s">
+      <c r="G45" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="12" t="s">
+    <row r="46" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B45" s="12">
+      <c r="B46" s="12">
         <v>1</v>
       </c>
-      <c r="G45" s="12" t="s">
+      <c r="G46" s="12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
+    <row r="47" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B46" s="12">
+      <c r="B47" s="12">
         <v>0</v>
       </c>
-      <c r="G46" s="12" t="s">
+      <c r="G47" s="12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="12" t="s">
+    <row r="48" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B47" s="12">
+      <c r="B48" s="12">
         <v>1</v>
       </c>
-      <c r="G47" s="12" t="s">
+      <c r="G48" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
+    <row r="49" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B49" s="8">
         <v>70</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="G49" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="I49" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>20</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>0</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G50" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>125</v>
       </c>
-      <c r="B50" s="13">
+      <c r="B51" s="13">
         <v>2000</v>
-      </c>
-      <c r="C50" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50">
-        <v>1990</v>
-      </c>
-      <c r="E50">
-        <v>2020</v>
-      </c>
-      <c r="G50" s="13" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>127</v>
-      </c>
-      <c r="B51" s="13">
-        <v>0.1</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
       </c>
       <c r="D51">
-        <v>0.05</v>
+        <v>1990</v>
       </c>
       <c r="E51">
-        <v>0.2</v>
+        <v>2020</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>129</v>
-      </c>
-      <c r="B52">
-        <v>0.75</v>
+        <v>127</v>
+      </c>
+      <c r="B52" s="13">
+        <v>0.1</v>
       </c>
       <c r="C52" t="s">
         <v>17</v>
       </c>
       <c r="D52">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="G52" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.2</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B53">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C53" t="s">
         <v>17</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
       <c r="G53" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54">
+        <v>0.5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="G54" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reasonavble priors for mixing params
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C96B78B-F169-3B4A-B96D-4FA29EB1493F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA7FE42-5074-554A-95A7-E55D7E6F0C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="2220" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -925,7 +925,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1006,7 +1006,7 @@
         <v>0.01</v>
       </c>
       <c r="E3" s="2">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>136</v>
@@ -1046,10 +1046,10 @@
         <v>17</v>
       </c>
       <c r="D5" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E5" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
Update priors and targets with latest data
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA7FE42-5074-554A-95A7-E55D7E6F0C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DA8488-D389-AE40-8B8F-12EAB899AB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="2220" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -924,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1625,16 +1625,16 @@
         <v>62</v>
       </c>
       <c r="B41" s="11">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="11">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E41" s="11">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="G41" s="11" t="s">
         <v>104</v>
@@ -1656,16 +1656,16 @@
         <v>55</v>
       </c>
       <c r="B43" s="11">
-        <v>0.4</v>
+        <v>0.85</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D43" s="11">
-        <v>0.5</v>
+        <v>0.72</v>
       </c>
       <c r="E43" s="11">
-        <v>1</v>
+        <v>0.93</v>
       </c>
       <c r="G43" s="11" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
Uncertainty around bcg effect
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DA8488-D389-AE40-8B8F-12EAB899AB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDA24E3-2157-A94D-82EC-FA7487995D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="139">
   <si>
     <t>parameter</t>
   </si>
@@ -924,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6C8F8-7718-2F41-B98B-2D455BE12E8B}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1110,6 +1110,15 @@
       </c>
       <c r="B8" s="4">
         <v>0.5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
Update trans rate prior
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrag0004/Documents/Code/tb_hierarchical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDA24E3-2157-A94D-82EC-FA7487995D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010D7A53-AEF9-0843-B602-262A52D9E1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D0791FB0-CE82-4F48-97F1-167D990A1A74}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -925,7 +925,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -980,10 +980,10 @@
         <v>17</v>
       </c>
       <c r="D2" s="2">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="E2" s="2">
-        <v>5.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>71</v>

</xml_diff>